<commit_message>
script to pick trade every 1/2/4 hours, and record it
</commit_message>
<xml_diff>
--- a/saved_model/results/1_h.xlsx
+++ b/saved_model/results/1_h.xlsx
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,6 +428,278 @@
         <v>4589</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>16.88810595718799</v>
+      </c>
+      <c r="C5">
+        <v>7.410636442894507</v>
+      </c>
+      <c r="D5">
+        <v>1.595419847328244</v>
+      </c>
+      <c r="E5">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-23.18958569898614</v>
+      </c>
+      <c r="C6">
+        <v>12.51362546326575</v>
+      </c>
+      <c r="D6">
+        <v>1.174242424242424</v>
+      </c>
+      <c r="E6">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>63.13150677758502</v>
+      </c>
+      <c r="C7">
+        <v>9.136502398604449</v>
+      </c>
+      <c r="D7">
+        <v>1.479289940828402</v>
+      </c>
+      <c r="E7">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>61.20206252164174</v>
+      </c>
+      <c r="C8">
+        <v>8.287895310796074</v>
+      </c>
+      <c r="D8">
+        <v>1.620689655172414</v>
+      </c>
+      <c r="E8">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>11.47957239204662</v>
+      </c>
+      <c r="C9">
+        <v>3.926701570680628</v>
+      </c>
+      <c r="D9">
+        <v>1.535211267605634</v>
+      </c>
+      <c r="E9">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>54.95367048012035</v>
+      </c>
+      <c r="C10">
+        <v>6.938686449923631</v>
+      </c>
+      <c r="D10">
+        <v>1.355555555555556</v>
+      </c>
+      <c r="E10">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>102.3194526587594</v>
+      </c>
+      <c r="C11">
+        <v>6.678306416412047</v>
+      </c>
+      <c r="D11">
+        <v>1.615384615384615</v>
+      </c>
+      <c r="E11">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>74.99318399046976</v>
+      </c>
+      <c r="C12">
+        <v>6.090373280943026</v>
+      </c>
+      <c r="D12">
+        <v>1.607476635514019</v>
+      </c>
+      <c r="E12">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>84.77249498106892</v>
+      </c>
+      <c r="C13">
+        <v>5.349344978165939</v>
+      </c>
+      <c r="D13">
+        <v>1.692307692307692</v>
+      </c>
+      <c r="E13">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>58.50058886331681</v>
+      </c>
+      <c r="C14">
+        <v>2.839047827036471</v>
+      </c>
+      <c r="D14">
+        <v>1.708333333333333</v>
+      </c>
+      <c r="E14">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>50.44483745362236</v>
+      </c>
+      <c r="C15">
+        <v>4.084753167321974</v>
+      </c>
+      <c r="D15">
+        <v>1.367088607594937</v>
+      </c>
+      <c r="E15">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>68.70088120721429</v>
+      </c>
+      <c r="C16">
+        <v>4.610006554511689</v>
+      </c>
+      <c r="D16">
+        <v>1.573170731707317</v>
+      </c>
+      <c r="E16">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>7.931818834894001</v>
+      </c>
+      <c r="C17">
+        <v>4.567307692307692</v>
+      </c>
+      <c r="D17">
+        <v>1.177083333333333</v>
+      </c>
+      <c r="E17">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>83.65057414842337</v>
+      </c>
+      <c r="C18">
+        <v>3.497267759562841</v>
+      </c>
+      <c r="D18">
+        <v>1.388059701492537</v>
+      </c>
+      <c r="E18">
+        <v>4575</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>16.64545044202842</v>
+      </c>
+      <c r="C19">
+        <v>3.279405334499344</v>
+      </c>
+      <c r="D19">
+        <v>1.238805970149254</v>
+      </c>
+      <c r="E19">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>-26.39520180019328</v>
+      </c>
+      <c r="C20">
+        <v>4.176689263065821</v>
+      </c>
+      <c r="D20">
+        <v>1.122222222222222</v>
+      </c>
+      <c r="E20">
+        <v>4573</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>